<commit_message>
Added calculation sheets for werkgebieden.
</commit_message>
<xml_diff>
--- a/docs/opdracht 4/werkgebieden/resources/Vdsat_scaling_calculation.xlsx
+++ b/docs/opdracht 4/werkgebieden/resources/Vdsat_scaling_calculation.xlsx
@@ -337,72 +337,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>9.2900000000000003E-4</v>
+        <v>9.3360000000000003E-4</v>
       </c>
       <c r="B1">
-        <v>1.5</v>
+        <v>1.51</v>
       </c>
       <c r="C1">
         <f>A1/POWER(B1,2)</f>
-        <v>4.1288888888888891E-4</v>
+        <v>4.0945572562606903E-4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>6.3699999999999998E-4</v>
+        <v>6.491E-4</v>
       </c>
       <c r="B2">
-        <v>1.3</v>
+        <v>1.335</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C5" si="0">A2/POWER(B2,2)</f>
-        <v>3.7692307692307689E-4</v>
+        <v>3.6420766177110072E-4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>3.7419999999999999E-4</v>
+        <v>3.8559999999999999E-4</v>
       </c>
       <c r="B3">
-        <v>1.05</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>3.3941043083900223E-4</v>
+        <v>3.1867768595041318E-4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1.604E-4</v>
+        <v>1.6310000000000001E-4</v>
       </c>
       <c r="B4">
-        <v>0.75</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>2.8515555555555554E-4</v>
+        <v>2.7155046826222681E-4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1.6140000000000001E-5</v>
+        <v>1.8349999999999999E-5</v>
       </c>
       <c r="B5">
-        <v>0.2</v>
+        <v>0.27</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>4.0349999999999994E-4</v>
+        <v>2.5171467764060351E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f>AVERAGE(C1:C5)</f>
+        <v>3.2312124385008265E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>